<commit_message>
- Updated RTM - Fixed numbering in SRS V0.6
Signed-off-by: mariam-elshakafi <mariam.elshakafi@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Specification/Traceability/PO3_DGW_RTM.xlsx
+++ b/Software Specification/Traceability/PO3_DGW_RTM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\iTi_Workspace\SE_Workspace\SWENG_PO3_DigitalWatch\Drafts\Mariam\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\iTi_Workspace\SE_Workspace\SWENG_PO3_DigitalWatch\Software Specification\Traceability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC648F5C-6115-493C-8663-517113DEED44}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDCF14C-44D1-4C59-A5F0-50B9F70AA108}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_Toc30870367" localSheetId="0">RTM!$A$6</definedName>
+    <definedName name="_Toc30870367" localSheetId="0">RTM!$A$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Have Problems</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Not answered</t>
   </si>
   <si>
-    <t>Answered</t>
-  </si>
-  <si>
     <t>Digital Watch - Requirement Tracability Matrix</t>
   </si>
   <si>
@@ -57,82 +54,157 @@
     <t>SRS ID</t>
   </si>
   <si>
-    <t>FUNC_PO3_DGW_CYRS_01_V01</t>
-  </si>
-  <si>
-    <t>FUNC_PO3_DGW_CYRS_02_V01</t>
-  </si>
-  <si>
-    <t>FUNC_PO3_DGW_CYRS_03_V01</t>
-  </si>
-  <si>
-    <t>FUNC_PO3_DGW_CYRS_04_V01</t>
-  </si>
-  <si>
-    <t>FUNC_PO3_DGW_CYRS_05_V01</t>
-  </si>
-  <si>
-    <t>FUNC_PO3_DGW_CYRS_06_V01</t>
-  </si>
-  <si>
-    <t>FUNC_PO3_DGW_CYRS_07_V02</t>
-  </si>
-  <si>
-    <t>FUNC_PO3_DGW_CYRS_08_V01</t>
-  </si>
-  <si>
-    <t>FUNC_PO3_DGW_CYRS_09_V01</t>
-  </si>
-  <si>
-    <t>Req_P03DGW_SRS_AdjustTime_001_V01</t>
-  </si>
-  <si>
-    <t>Req_P03DGW_SRS_AdjustTime_002_V01</t>
-  </si>
-  <si>
-    <t>Req_P03DGW_SRS_AdjustTime_003_V01</t>
-  </si>
-  <si>
-    <t>Req_P03DGW_SRS_AdjustTime_004_V01</t>
-  </si>
-  <si>
-    <t>Req_P03DGW_SRS_DisplayTime_001_V01</t>
-  </si>
-  <si>
-    <t>Req_P03DGW_SRS_DisplayTime_002_V01</t>
-  </si>
-  <si>
-    <t>Req_P03DGW_SRS_AlarmMode_001_V01</t>
-  </si>
-  <si>
-    <t>Req_P03DGW_SRS_AlarmMode_002_V01</t>
-  </si>
-  <si>
-    <t>Req_P03DGW_SRS_AlarmMode_003_V01</t>
-  </si>
-  <si>
-    <t>Req_P03DGW_SRS_AlarmMode_004_V01</t>
-  </si>
-  <si>
-    <t>Req_P03DGW_SRS_AlarmMode_005_V01</t>
-  </si>
-  <si>
-    <t>Req_P03DGW_SRS_AlarmMode_006_V01</t>
-  </si>
-  <si>
-    <t>Req_P03DGW_SRS_StopWatchMode_001_V01</t>
-  </si>
-  <si>
-    <t>Req_P03DGW_SRS_StopWatchMode_002_V01</t>
-  </si>
-  <si>
-    <t>Req_P03DGW_SRS_StopWatchMode_003_V02</t>
-  </si>
-  <si>
-    <t>Req_P03DGW_SRS_StopWatchMode_004_V01</t>
-  </si>
-  <si>
-    <t>Req_P03DGW_SRS_StopWatchMode_005_V01</t>
+    <t>REQ_PO3_DGW_CYRS_01_V02</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_001_V05</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_002_V05</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_003_V05</t>
+  </si>
+  <si>
+    <t>REQ_PO3_DGW_CYRS_02_V02</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_004_V05</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_006_V05</t>
+  </si>
+  <si>
+    <t>REQ_PO3_DGW_CYRS_04_V02</t>
+  </si>
+  <si>
+    <t>REQ_PO3_DGW_CYRS_03_V02</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_007_V05</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_008_V05</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_009_V05</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_010_V05</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_011_V05</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_012_V05</t>
+  </si>
+  <si>
+    <t>FUNC_PO3_DGW_CYRS_05_V02</t>
+  </si>
+  <si>
+    <t>FUNC_PO3_DGW_CYRS_06_V02</t>
+  </si>
+  <si>
+    <t>FUNC_PO3_DGW_CYRS_07_V03</t>
+  </si>
+  <si>
+    <t>FUNC_PO3_DGW_CYRS_08_V02</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_013_V04</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_005_V04</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_014_V05</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_015_V05</t>
+  </si>
+  <si>
+    <t>FUNC_PO3_DGW_CYRS_09_V02</t>
+  </si>
+  <si>
+    <t>FUNC_PO3_DGW_CYRS_10_V01</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_016_V05</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_017_V05</t>
+  </si>
+  <si>
+    <t>REQ_PO3_DGW_CYRS_11_V01</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_018_V05</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_019_V05</t>
+  </si>
+  <si>
+    <t>REQ_PO3_DGW_CYRS_12_V01</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_020_V05</t>
+  </si>
+  <si>
+    <t>REQ_PO3_DGW_CYRS_13_V01</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_021_V05</t>
+  </si>
+  <si>
+    <t>REQ_PO3_DGW_CYRS_14_V01</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_022_V05</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_023_V05</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_024_V04</t>
+  </si>
+  <si>
+    <t>REQ_PO3_DGW_CYRS_16_V01</t>
+  </si>
+  <si>
+    <t>REQ_PO3_DGW_CYRS_15_V01</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_025_V04</t>
+  </si>
+  <si>
+    <t>REQ_PO3_DGW_CYRS_17_V01</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_026_V05</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_027_V01</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_028_V01</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_029_V01</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_030_V01</t>
+  </si>
+  <si>
+    <t>REQ_PO3_DGW_CYRS_18_V01</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_031_V01</t>
+  </si>
+  <si>
+    <t>Req_P03DGW_SRS_032_V01</t>
+  </si>
+  <si>
+    <t>REQ_PO3_DGW_CYRS_19_V01</t>
   </si>
 </sst>
 </file>
@@ -412,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -432,6 +504,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -441,50 +555,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -821,24 +902,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="24"/>
+    </row>
+    <row r="2" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="19"/>
+    </row>
+    <row r="3" spans="1:5" s="4" customFormat="1" ht="19.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="23"/>
-    </row>
-    <row r="2" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="24"/>
-    </row>
-    <row r="3" spans="1:5" s="4" customFormat="1" ht="19.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
+      <c r="B3" s="18" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>6</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="4" t="s">
@@ -846,11 +927,11 @@
       </c>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>20</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="6" t="s">
@@ -859,277 +940,321 @@
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="11"/>
-      <c r="B5" s="14" t="s">
-        <v>21</v>
+      <c r="A5" s="20"/>
+      <c r="B5" s="16" t="s">
+        <v>8</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>16</v>
+      <c r="A6" s="20"/>
+      <c r="B6" s="10" t="s">
+        <v>9</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="11"/>
-      <c r="B7" s="17" t="s">
-        <v>17</v>
+      <c r="A7" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="11"/>
-      <c r="B8" s="19" t="s">
-        <v>18</v>
+      <c r="A8" s="20"/>
+      <c r="B8" s="13" t="s">
+        <v>26</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="6" t="s">
-        <v>3</v>
-      </c>
+      <c r="D8" s="6"/>
       <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="11"/>
-      <c r="B9" s="18" t="s">
-        <v>19</v>
+      <c r="A9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>22</v>
+      <c r="A10" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>23</v>
+      <c r="A11" s="20"/>
+      <c r="B11" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="11"/>
-      <c r="B12" s="19" t="s">
-        <v>24</v>
+    <row r="12" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="11"/>
-      <c r="B13" s="20" t="s">
-        <v>25</v>
+    <row r="13" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="26"/>
+      <c r="B13" s="13" t="s">
+        <v>18</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="11"/>
-      <c r="B14" s="15" t="s">
-        <v>26</v>
+      <c r="A14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>27</v>
+      <c r="A15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="16" t="s">
+      <c r="A16" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="26"/>
+      <c r="B18" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="11"/>
-      <c r="B17" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="12" t="s">
+    </row>
+    <row r="19" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="17" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="12" t="s">
+    <row r="20" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="26"/>
+      <c r="B20" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-    </row>
-    <row r="22" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-    </row>
-    <row r="23" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-    </row>
-    <row r="24" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-    </row>
-    <row r="25" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-    </row>
-    <row r="26" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-    </row>
-    <row r="27" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-    </row>
-    <row r="28" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-    </row>
-    <row r="29" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-    </row>
-    <row r="30" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-    </row>
-    <row r="31" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-    </row>
-    <row r="32" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
+    <row r="21" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="26"/>
+      <c r="B22" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="26"/>
+      <c r="B26" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="27"/>
+      <c r="B30" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="27"/>
+      <c r="B31" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="27"/>
+      <c r="B32" s="8" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="33" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="8" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="34" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
+      <c r="A34" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="35" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
+      <c r="A35" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="36" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
     </row>
     <row r="37" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
     </row>
     <row r="38" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
     </row>
     <row r="39" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
     </row>
     <row r="40" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
     </row>
     <row r="41" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
     </row>
     <row r="42" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
     </row>
     <row r="43" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
     </row>
     <row r="44" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
     </row>
     <row r="45" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
     </row>
     <row r="46" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12"/>
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
     </row>
     <row r="47" spans="1:2" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12"/>
+      <c r="A47" s="8"/>
+      <c r="B47" s="8"/>
     </row>
     <row r="48" spans="1:2" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A16:A17"/>
+  <mergeCells count="11">
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A29:A33"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>